<commit_message>
started adding questions to the database
</commit_message>
<xml_diff>
--- a/data_base/other_files/PytaniaProjekt.xlsx
+++ b/data_base/other_files/PytaniaProjekt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damia\Desktop\Trivia_Game\data_base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damia\Desktop\Trivia_Game\data_base\other_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611A1A5C-47C3-4901-B6DD-4FB9B0973135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997763C8-ADEE-439D-982C-08AC9A87A9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6141DBD3-99C8-4C1A-8268-ADC8A4714638}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{6141DBD3-99C8-4C1A-8268-ADC8A4714638}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,36 +25,219 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
-  <si>
-    <t>odpowiedz poprawna</t>
-  </si>
-  <si>
-    <t>odpowiedz2</t>
-  </si>
-  <si>
-    <t>odpowiedz3</t>
-  </si>
-  <si>
-    <t>kategoria</t>
-  </si>
-  <si>
-    <t>sport</t>
-  </si>
-  <si>
-    <t>1:1</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>W jakim klubie gra Robert Lewandowski?</t>
-  </si>
-  <si>
-    <t>pytanie (max 80 znakow)</t>
-  </si>
-  <si>
-    <t>max 26 znakow odpowiedzi</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+  <si>
+    <t>Który władca nosił najbardziej modny strój na bitwie pod Waterloo?</t>
+  </si>
+  <si>
+    <t>Napoleon Bonaparte</t>
+  </si>
+  <si>
+    <t>Juliusz Cezar</t>
+  </si>
+  <si>
+    <t>Kleopatra</t>
+  </si>
+  <si>
+    <t>Neil Armstrong</t>
+  </si>
+  <si>
+    <t>Kto był pierwszym prezydentem Stanów Zjednoczonych?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> George Washington</t>
+  </si>
+  <si>
+    <t>Abraham Lincoln</t>
+  </si>
+  <si>
+    <t>Thomas Jefferson</t>
+  </si>
+  <si>
+    <t>Donald Trump</t>
+  </si>
+  <si>
+    <t>Który wynalazek był kluczowy dla rewolucji przemysłowej w XIX wieku?</t>
+  </si>
+  <si>
+    <t>Maszyna parowa</t>
+  </si>
+  <si>
+    <t>Elektryczność</t>
+  </si>
+  <si>
+    <t>Telegraf</t>
+  </si>
+  <si>
+    <t>Silnik spalinowy</t>
+  </si>
+  <si>
+    <t>W którym roku odkryto Amerykę?</t>
+  </si>
+  <si>
+    <t>W jakich latach trwała I wojna światowa?</t>
+  </si>
+  <si>
+    <t>1914–1918</t>
+  </si>
+  <si>
+    <t>1939–1945</t>
+  </si>
+  <si>
+    <t>1871–1878</t>
+  </si>
+  <si>
+    <t>1919–1923</t>
+  </si>
+  <si>
+    <t>Po co kibicowi reprezentacji Polski szalik?</t>
+  </si>
+  <si>
+    <t>Do wycierania łez</t>
+  </si>
+  <si>
+    <t>Bo jest zimno</t>
+  </si>
+  <si>
+    <t>Bo jest wiernynm kibicem</t>
+  </si>
+  <si>
+    <t>Bo Polska to jego ojczyzna</t>
+  </si>
+  <si>
+    <t>Które z tych zwrotów jest związane z golfem?</t>
+  </si>
+  <si>
+    <t>Birdie</t>
+  </si>
+  <si>
+    <t>Slam dunk</t>
+  </si>
+  <si>
+    <t>Touchdown</t>
+  </si>
+  <si>
+    <t>Home run</t>
+  </si>
+  <si>
+    <t>Kto jest rekordzistą wszech czasów w biegu na 100 metrów?</t>
+  </si>
+  <si>
+    <t>Usain Bolt</t>
+  </si>
+  <si>
+    <t>Carl Lewis</t>
+  </si>
+  <si>
+    <t>Jesse Owens</t>
+  </si>
+  <si>
+    <t>Asafa Powell</t>
+  </si>
+  <si>
+    <t>Który kierowca Formuły 1 zdobył najwięcej tytułów mistrza świata?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lewis Hamilton</t>
+  </si>
+  <si>
+    <t>Ayrton Senna</t>
+  </si>
+  <si>
+    <t>Michael Schumacher</t>
+  </si>
+  <si>
+    <t>Max Verstappen</t>
+  </si>
+  <si>
+    <t>Który kraj był gospodarzem Mistrzostw Świata w piłce nożnej w 2014 roku?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brazylia </t>
+  </si>
+  <si>
+    <t>Niemcy</t>
+  </si>
+  <si>
+    <t>Argentyna</t>
+  </si>
+  <si>
+    <t>Francja</t>
+  </si>
+  <si>
+    <t>Jaka jest najlepsza rada dla programisty?</t>
+  </si>
+  <si>
+    <t>Jeśli działa, nie dotykaj</t>
+  </si>
+  <si>
+    <t>Bądź Cierpliwy i Kreatywny</t>
+  </si>
+  <si>
+    <t>Zbuduj Portfolio</t>
+  </si>
+  <si>
+    <t>Rób dokładną dokumentację</t>
+  </si>
+  <si>
+    <t>Jak nazywa się system kodowania tekstu, który obejmuje znaki z różnych języków?</t>
+  </si>
+  <si>
+    <t>Unicode</t>
+  </si>
+  <si>
+    <t>Multicode</t>
+  </si>
+  <si>
+    <t>Policode</t>
+  </si>
+  <si>
+    <t>Supercode</t>
+  </si>
+  <si>
+    <t>Co oznacza skrót SSD w kontekście pamięci komputerowej?</t>
+  </si>
+  <si>
+    <t>Solid State Drive</t>
+  </si>
+  <si>
+    <t>Super Speed Drive</t>
+  </si>
+  <si>
+    <t>System Storage Device</t>
+  </si>
+  <si>
+    <t>Speedy Software Dev</t>
+  </si>
+  <si>
+    <t>Jakie polecenie używane jest do powrotu do poprzedniego katalogu w Linuxie?</t>
+  </si>
+  <si>
+    <t>cd ..</t>
+  </si>
+  <si>
+    <t>cd back</t>
+  </si>
+  <si>
+    <t>cd return</t>
+  </si>
+  <si>
+    <t>go back</t>
+  </si>
+  <si>
+    <t>Co oznacza skrót LAN w kontekście sieci komputerowych?</t>
+  </si>
+  <si>
+    <t>Local Area Network</t>
+  </si>
+  <si>
+    <t>Large Access Node</t>
+  </si>
+  <si>
+    <t>Long Analog Network</t>
+  </si>
+  <si>
+    <t>Last Authentication Node</t>
   </si>
 </sst>
 </file>
@@ -112,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -120,6 +303,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -436,311 +622,468 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE2B563-E523-4F70-9BE4-817456DC8DAD}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="171" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="4"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2">
-        <v>4.2361111111111106E-2</v>
-      </c>
-      <c r="F2" s="2">
-        <v>8.5416666666666655E-2</v>
-      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="E3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="G3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="B6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1492</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1500</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1607</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1776</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>15</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>

</xml_diff>